<commit_message>
Login and Signup Readers - MultiAuth
</commit_message>
<xml_diff>
--- a/public/uploads/reader.xlsx
+++ b/public/uploads/reader.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
   <si>
     <t>ID</t>
   </si>
@@ -37,91 +37,133 @@
     <t>facebook</t>
   </si>
   <si>
+    <t>UIT</t>
+  </si>
+  <si>
+    <t>17521109</t>
+  </si>
+  <si>
     <t>Lê Phan Vũ Thuận</t>
   </si>
   <si>
+    <t>17521109@gm.uit.edu.vn</t>
+  </si>
+  <si>
+    <t>17520328</t>
+  </si>
+  <si>
     <t>Trần Quang Đạo</t>
   </si>
   <si>
+    <t>17520328@gm.uit.edu.vn</t>
+  </si>
+  <si>
+    <t>16521084</t>
+  </si>
+  <si>
     <t>Trần Đình Tạo</t>
   </si>
   <si>
+    <t>trandinhtao1998@gmail.com</t>
+  </si>
+  <si>
+    <t>17520702</t>
+  </si>
+  <si>
     <t>Nguyễn Huỳnh Lợi</t>
   </si>
   <si>
+    <t>17520702@gm.uit.edu.vn</t>
+  </si>
+  <si>
+    <t>16520191</t>
+  </si>
+  <si>
     <t>Nguyễn Hữu Đạt</t>
   </si>
   <si>
+    <t>16520191@gm.uit.edu.vn</t>
+  </si>
+  <si>
+    <t>17520926</t>
+  </si>
+  <si>
     <t>Nguyễn Thị Bích Phượng</t>
   </si>
   <si>
+    <t>17520926@gm.uit.edu.vn</t>
+  </si>
+  <si>
+    <t>1656030112</t>
+  </si>
+  <si>
     <t>Trần Thị Như Quỳnh</t>
   </si>
   <si>
+    <t>USSH</t>
+  </si>
+  <si>
+    <t>trannhuquynhbck16@gmail.com</t>
+  </si>
+  <si>
+    <t>1756110054</t>
+  </si>
+  <si>
     <t>Lê Huỳnh Tuyết Hương</t>
   </si>
   <si>
+    <t>toilamotmauxanh@gmail.com</t>
+  </si>
+  <si>
+    <t>17520452</t>
+  </si>
+  <si>
     <t>Vũ Anh Hào</t>
   </si>
   <si>
+    <t>17520452@gm.uit.edu.vn</t>
+  </si>
+  <si>
+    <t>17521295</t>
+  </si>
+  <si>
     <t>Cáp Hữu Anh Đức</t>
   </si>
   <si>
+    <t>ken.manucian.125@gmail.com</t>
+  </si>
+  <si>
+    <t>14520786</t>
+  </si>
+  <si>
     <t>Phùng Thanh Tài</t>
   </si>
   <si>
+    <t>taipt1301@gmail.com</t>
+  </si>
+  <si>
+    <t>1757060071</t>
+  </si>
+  <si>
     <t>Nguyễn Thị Mai Lan</t>
   </si>
   <si>
+    <t>nhoklan89810@gmail.com</t>
+  </si>
+  <si>
+    <t>16520373</t>
+  </si>
+  <si>
     <t>Đặng Văn Hiệp</t>
   </si>
   <si>
+    <t>16520373@gm.uit.edu.vn</t>
+  </si>
+  <si>
+    <t>17520929</t>
+  </si>
+  <si>
     <t>Phan Lê Kim Phượng</t>
-  </si>
-  <si>
-    <t>UIT</t>
-  </si>
-  <si>
-    <t>USSH</t>
-  </si>
-  <si>
-    <t>17521109@gm.uit.edu.vn</t>
-  </si>
-  <si>
-    <t>17520328@gm.uit.edu.vn</t>
-  </si>
-  <si>
-    <t>trandinhtao1998@gmail.com</t>
-  </si>
-  <si>
-    <t>17520702@gm.uit.edu.vn</t>
-  </si>
-  <si>
-    <t>16520191@gm.uit.edu.vn</t>
-  </si>
-  <si>
-    <t>17520926@gm.uit.edu.vn</t>
-  </si>
-  <si>
-    <t>trannhuquynhbck16@gmail.com</t>
-  </si>
-  <si>
-    <t>toilamotmauxanh@gmail.com</t>
-  </si>
-  <si>
-    <t>17520452@gm.uit.edu.vn</t>
-  </si>
-  <si>
-    <t>ken.manucian.125@gmail.com</t>
-  </si>
-  <si>
-    <t>taipt1301@gmail.com</t>
-  </si>
-  <si>
-    <t>nhoklan89810@gmail.com</t>
-  </si>
-  <si>
-    <t>16520373@gm.uit.edu.vn</t>
   </si>
   <si>
     <t>17520929@gm.uit.edu.vn</t>
@@ -131,7 +173,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -143,19 +185,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -165,7 +194,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -173,87 +202,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,19 +510,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A2" sqref="A2:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.75" customWidth="1"/>
-    <col min="2" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="3" width="29.375" customWidth="1"/>
-    <col min="5" max="5" width="23.625" customWidth="1"/>
-    <col min="6" max="6" width="17.375" customWidth="1"/>
+    <col min="6" max="6" width="14.375" customWidth="1"/>
     <col min="7" max="7" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -600,19 +551,19 @@
       <c r="A2">
         <v>16</v>
       </c>
-      <c r="B2" s="3">
-        <v>17521109</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="12">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2">
         <v>1635162579</v>
       </c>
     </row>
@@ -620,19 +571,19 @@
       <c r="A3">
         <v>17</v>
       </c>
-      <c r="B3" s="3">
-        <v>17520328</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="12">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3">
         <v>1673599258</v>
       </c>
     </row>
@@ -640,19 +591,19 @@
       <c r="A4">
         <v>18</v>
       </c>
-      <c r="B4" s="3">
-        <v>16521084</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="12">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4">
         <v>1673206562</v>
       </c>
     </row>
@@ -660,19 +611,19 @@
       <c r="A5">
         <v>19</v>
       </c>
-      <c r="B5" s="3">
-        <v>17520702</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="12">
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5">
         <v>961178682</v>
       </c>
     </row>
@@ -680,19 +631,19 @@
       <c r="A6">
         <v>20</v>
       </c>
-      <c r="B6" s="3">
-        <v>16520191</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="9" t="s">
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="12">
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6">
         <v>1629480055</v>
       </c>
     </row>
@@ -700,19 +651,19 @@
       <c r="A7">
         <v>21</v>
       </c>
-      <c r="B7" s="3">
-        <v>17520926</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="12">
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7">
         <v>914129953</v>
       </c>
     </row>
@@ -720,19 +671,19 @@
       <c r="A8">
         <v>22</v>
       </c>
-      <c r="B8" s="3">
-        <v>1656030112</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8">
         <v>973003935</v>
       </c>
     </row>
@@ -740,19 +691,19 @@
       <c r="A9">
         <v>23</v>
       </c>
-      <c r="B9" s="3">
-        <v>1756110054</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="B9" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="12">
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9">
         <v>919177427</v>
       </c>
     </row>
@@ -760,19 +711,19 @@
       <c r="A10">
         <v>24</v>
       </c>
-      <c r="B10" s="3">
-        <v>17520452</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="12">
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10">
         <v>928291447</v>
       </c>
     </row>
@@ -780,19 +731,19 @@
       <c r="A11">
         <v>25</v>
       </c>
-      <c r="B11" s="3">
-        <v>17521295</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="12">
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11">
         <v>1245248345</v>
       </c>
     </row>
@@ -800,19 +751,19 @@
       <c r="A12">
         <v>26</v>
       </c>
-      <c r="B12" s="3">
-        <v>14520786</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="12">
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12">
         <v>961118679</v>
       </c>
     </row>
@@ -820,19 +771,19 @@
       <c r="A13">
         <v>27</v>
       </c>
-      <c r="B13" s="4">
-        <v>1757060071</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="13">
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13">
         <v>1692895398</v>
       </c>
     </row>
@@ -840,19 +791,19 @@
       <c r="A14">
         <v>28</v>
       </c>
-      <c r="B14" s="3">
-        <v>16520373</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="12">
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14">
         <v>1237897572</v>
       </c>
     </row>
@@ -860,28 +811,21 @@
       <c r="A15">
         <v>29</v>
       </c>
-      <c r="B15" s="3">
-        <v>17520929</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="12">
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15">
         <v>934034906</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>